<commit_message>
commit open new account test case
</commit_message>
<xml_diff>
--- a/Data Files/Test data.xlsx
+++ b/Data Files/Test data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6800" activeTab="1"/>
+    <workbookView windowWidth="19200" windowHeight="6800"/>
   </bookViews>
   <sheets>
     <sheet name="Sign up" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
     <t>0564411666</t>
   </si>
   <si>
-    <t>madboly1</t>
+    <t>madboly5</t>
   </si>
   <si>
     <t>510520@Mm</t>
@@ -1039,8 +1039,8 @@
   <sheetPr/>
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="6"/>
@@ -1163,7 +1163,7 @@
   <sheetPr/>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
some enahncement in open new account test case
</commit_message>
<xml_diff>
--- a/Data Files/Test data.xlsx
+++ b/Data Files/Test data.xlsx
@@ -81,7 +81,7 @@
     <t>0564411666</t>
   </si>
   <si>
-    <t>madboly1</t>
+    <t>madboly3</t>
   </si>
   <si>
     <t>510520@Mm</t>
@@ -1040,7 +1040,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="6"/>

</xml_diff>

<commit_message>
implement bill pay test case
</commit_message>
<xml_diff>
--- a/Data Files/Test data.xlsx
+++ b/Data Files/Test data.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Sign up" sheetId="1" r:id="rId1"/>
     <sheet name="General Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Pay bill" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>First Name</t>
   </si>
@@ -81,7 +82,7 @@
     <t>0564411666</t>
   </si>
   <si>
-    <t>madboly10</t>
+    <t>username1</t>
   </si>
   <si>
     <t>510520@Mm</t>
@@ -93,7 +94,40 @@
     <t>Transfer amount</t>
   </si>
   <si>
+    <t>Account Created Success Message</t>
+  </si>
+  <si>
     <t>https://parabank.parasoft.com/</t>
+  </si>
+  <si>
+    <t>Congratulations, your account is now open.</t>
+  </si>
+  <si>
+    <t>Payee Name</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Verify Account</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Sucees Message</t>
+  </si>
+  <si>
+    <t>Mahmoud Elsayed</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>0564151658</t>
+  </si>
+  <si>
+    <t>Bill Payment Complete</t>
   </si>
 </sst>
 </file>
@@ -714,8 +748,9 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
@@ -1043,7 +1078,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="6"/>
@@ -1062,51 +1097,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E2" t="s">
@@ -1115,7 +1150,7 @@
       <c r="F2">
         <v>1234</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="6" t="s">
         <v>16</v>
       </c>
       <c r="H2">
@@ -1124,32 +1159,32 @@
       <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1164,31 +1199,131 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
     <col min="2" max="2" width="16.2727272727273" customWidth="1"/>
+    <col min="3" max="3" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>20</v>
       </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="17.9090909090909" customWidth="1"/>
+    <col min="2" max="2" width="8.63636363636364" customWidth="1"/>
+    <col min="3" max="3" width="7.18181818181818" customWidth="1"/>
+    <col min="4" max="4" width="6" customWidth="1"/>
+    <col min="5" max="5" width="9.09090909090909" customWidth="1"/>
+    <col min="6" max="6" width="11.8181818181818" customWidth="1"/>
+    <col min="7" max="7" width="8.63636363636364" customWidth="1"/>
+    <col min="8" max="8" width="14.7272727272727" customWidth="1"/>
+    <col min="9" max="9" width="8.18181818181818" customWidth="1"/>
+    <col min="10" max="10" width="21.4545454545455" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2">
+        <v>1234</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2">
+        <v>12345</v>
+      </c>
+      <c r="H2">
+        <v>12345</v>
+      </c>
+      <c r="I2">
+        <v>20</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
start with find transactions test scenario
</commit_message>
<xml_diff>
--- a/Data Files/Test data.xlsx
+++ b/Data Files/Test data.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6800"/>
+    <workbookView windowWidth="19200" windowHeight="6800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sign up" sheetId="1" r:id="rId1"/>
     <sheet name="General Data" sheetId="2" r:id="rId2"/>
     <sheet name="Pay bill" sheetId="3" r:id="rId3"/>
+    <sheet name="test" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>First Name</t>
   </si>
@@ -95,6 +96,12 @@
   </si>
   <si>
     <t>Account Created Success Message</t>
+  </si>
+  <si>
+    <t>Transaction date from</t>
+  </si>
+  <si>
+    <t>Transaction date to</t>
   </si>
   <si>
     <t>https://parabank.parasoft.com/</t>
@@ -748,9 +755,8 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
@@ -1077,7 +1083,7 @@
   <sheetPr/>
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
@@ -1097,51 +1103,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E2" t="s">
@@ -1150,7 +1156,7 @@
       <c r="F2">
         <v>1234</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H2">
@@ -1159,32 +1165,32 @@
       <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1199,19 +1205,20 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H7:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="4"/>
   <cols>
     <col min="2" max="2" width="16.2727272727273" customWidth="1"/>
     <col min="3" max="3" width="41" customWidth="1"/>
+    <col min="4" max="5" width="21.2727272727273" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1220,17 +1227,23 @@
       </c>
       <c r="C1" t="s">
         <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B2">
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1264,7 +1277,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1282,21 +1295,21 @@
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
@@ -1305,13 +1318,13 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E2">
         <v>1234</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>31</v>
+      <c r="F2" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="G2">
         <v>12345</v>
@@ -1322,12 +1335,28 @@
       <c r="I2">
         <v>20</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>32</v>
+      <c r="J2" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Working on find transaction test scenarios
</commit_message>
<xml_diff>
--- a/Data Files/Test data.xlsx
+++ b/Data Files/Test data.xlsx
@@ -83,7 +83,7 @@
     <t>0564411666</t>
   </si>
   <si>
-    <t>username1</t>
+    <t>username113</t>
   </si>
   <si>
     <t>510520@Mm</t>
@@ -755,9 +755,10 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
@@ -1084,7 +1085,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="6"/>
@@ -1138,16 +1139,16 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E2" t="s">
@@ -1156,7 +1157,7 @@
       <c r="F2">
         <v>1234</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="6" t="s">
         <v>16</v>
       </c>
       <c r="H2">
@@ -1165,32 +1166,32 @@
       <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1208,7 +1209,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H7:H8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="4"/>
@@ -1235,7 +1236,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1244,6 +1245,9 @@
       </c>
       <c r="C2" t="s">
         <v>25</v>
+      </c>
+      <c r="D2" s="2">
+        <v>45772</v>
       </c>
     </row>
   </sheetData>
@@ -1323,7 +1327,7 @@
       <c r="E2">
         <v>1234</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>33</v>
       </c>
       <c r="G2">
@@ -1335,7 +1339,7 @@
       <c r="I2">
         <v>20</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="6" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
workomg on find transaction scenario
</commit_message>
<xml_diff>
--- a/Data Files/Test data.xlsx
+++ b/Data Files/Test data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6800" activeTab="1"/>
+    <workbookView windowWidth="19200" windowHeight="6800"/>
   </bookViews>
   <sheets>
     <sheet name="Sign up" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>First Name</t>
   </si>
@@ -83,7 +83,7 @@
     <t>0564411666</t>
   </si>
   <si>
-    <t>username113</t>
+    <t>username126</t>
   </si>
   <si>
     <t>510520@Mm</t>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Congratulations, your account is now open.</t>
+  </si>
+  <si>
+    <t>4/28/2025</t>
   </si>
   <si>
     <t>Payee Name</t>
@@ -758,7 +761,7 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
@@ -1084,7 +1087,7 @@
   <sheetPr/>
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -1208,8 +1211,8 @@
   <sheetPr/>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="4"/>
@@ -1246,8 +1249,8 @@
       <c r="C2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="2">
-        <v>45772</v>
+      <c r="D2" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1281,7 +1284,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1299,21 +1302,21 @@
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
@@ -1322,13 +1325,13 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E2">
         <v>1234</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G2">
         <v>12345</v>
@@ -1340,7 +1343,7 @@
         <v>20</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
enhance keyword method 'updateProfileInfo mehtod'
</commit_message>
<xml_diff>
--- a/Data Files/Test data.xlsx
+++ b/Data Files/Test data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6800" activeTab="5"/>
+    <workbookView windowWidth="19200" windowHeight="6800"/>
   </bookViews>
   <sheets>
     <sheet name="Sign up" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,6 @@
     <sheet name="Pay bill" sheetId="3" r:id="rId3"/>
     <sheet name="Find transaction" sheetId="4" r:id="rId4"/>
     <sheet name="Open new account" sheetId="5" r:id="rId5"/>
-    <sheet name="Update profile" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>First Name</t>
   </si>
@@ -85,12 +84,36 @@
     <t>0564411666</t>
   </si>
   <si>
-    <t>username191</t>
+    <t>testuser5</t>
   </si>
   <si>
     <t>510520@Mm</t>
   </si>
   <si>
+    <t>ahmed</t>
+  </si>
+  <si>
+    <t>ali</t>
+  </si>
+  <si>
+    <t>mohamed</t>
+  </si>
+  <si>
+    <t>sayed</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>Cairo</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>0564411611</t>
+  </si>
+  <si>
     <t>End point</t>
   </si>
   <si>
@@ -116,9 +139,6 @@
   </si>
   <si>
     <t>Mahmoud Elsayed</t>
-  </si>
-  <si>
-    <t>state</t>
   </si>
   <si>
     <t>0564151658</t>
@@ -774,8 +794,8 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
@@ -1101,8 +1121,8 @@
   <sheetPr/>
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="6"/>
@@ -1113,45 +1133,45 @@
     <col min="4" max="4" width="4.90909090909091" customWidth="1"/>
     <col min="5" max="5" width="6" customWidth="1"/>
     <col min="6" max="6" width="9.09090909090909" customWidth="1"/>
-    <col min="7" max="7" width="7" customWidth="1"/>
-    <col min="8" max="8" width="5.18181818181818" customWidth="1"/>
+    <col min="7" max="7" width="11.8181818181818" customWidth="1"/>
+    <col min="8" max="8" width="8.54545454545454" customWidth="1"/>
     <col min="9" max="9" width="10.2727272727273" customWidth="1"/>
     <col min="10" max="10" width="10" customWidth="1"/>
     <col min="11" max="11" width="8.36363636363636" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1191,16 +1211,37 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+    <row r="4" spans="1:7">
+      <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4">
+        <v>4444</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3"/>
@@ -1231,6 +1272,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="4"/>
   <cols>
+    <col min="1" max="1" width="30.7272727272727" customWidth="1"/>
     <col min="2" max="2" width="16.2727272727273" customWidth="1"/>
     <col min="3" max="3" width="41" customWidth="1"/>
     <col min="4" max="5" width="21.2727272727273" customWidth="1"/>
@@ -1238,21 +1280,21 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>20</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1284,40 +1326,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>25</v>
+      <c r="G1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="J1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
@@ -1326,13 +1368,13 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E2">
         <v>1234</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="G2">
         <v>12345</v>
@@ -1344,7 +1386,7 @@
         <v>20</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1373,36 +1415,36 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
         <v>20</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>36</v>
+      <c r="B2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1417,7 +1459,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1"/>
@@ -1427,55 +1469,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="7"/>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implementing request a new loan test case
</commit_message>
<xml_diff>
--- a/Data Files/Test data.xlsx
+++ b/Data Files/Test data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6800"/>
+    <workbookView windowWidth="28800" windowHeight="12180" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sign up" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Pay bill" sheetId="3" r:id="rId3"/>
     <sheet name="Find transaction" sheetId="4" r:id="rId4"/>
     <sheet name="Open new account" sheetId="5" r:id="rId5"/>
+    <sheet name="Update profile info" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
   <si>
     <t>First Name</t>
   </si>
@@ -172,6 +173,12 @@
   </si>
   <si>
     <t>Account created success message</t>
+  </si>
+  <si>
+    <t>Update info_success message</t>
+  </si>
+  <si>
+    <t>Profile Updated</t>
   </si>
 </sst>
 </file>
@@ -184,7 +191,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +204,12 @@
       <sz val="9.75"/>
       <color rgb="FF5F7A77"/>
       <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Courier New"/>
       <charset val="134"/>
     </font>
     <font>
@@ -662,143 +675,144 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1121,71 +1135,71 @@
   <sheetPr/>
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="10.7272727272727" customWidth="1"/>
-    <col min="3" max="3" width="8.63636363636364" customWidth="1"/>
-    <col min="4" max="4" width="4.90909090909091" customWidth="1"/>
+    <col min="2" max="2" width="10.7238095238095" customWidth="1"/>
+    <col min="3" max="3" width="8.63809523809524" customWidth="1"/>
+    <col min="4" max="4" width="4.90476190476191" customWidth="1"/>
     <col min="5" max="5" width="6" customWidth="1"/>
-    <col min="6" max="6" width="9.09090909090909" customWidth="1"/>
-    <col min="7" max="7" width="11.8181818181818" customWidth="1"/>
-    <col min="8" max="8" width="8.54545454545454" customWidth="1"/>
-    <col min="9" max="9" width="10.2727272727273" customWidth="1"/>
+    <col min="6" max="6" width="9.09523809523809" customWidth="1"/>
+    <col min="7" max="7" width="11.8190476190476" customWidth="1"/>
+    <col min="8" max="8" width="8.54285714285714" customWidth="1"/>
+    <col min="9" max="9" width="10.2761904761905" customWidth="1"/>
     <col min="10" max="10" width="10" customWidth="1"/>
-    <col min="11" max="11" width="8.36363636363636" customWidth="1"/>
+    <col min="11" max="11" width="8.36190476190476" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E2" t="s">
@@ -1194,7 +1208,7 @@
       <c r="F2">
         <v>1234</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>16</v>
       </c>
       <c r="H2">
@@ -1203,34 +1217,34 @@
       <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E4" t="s">
@@ -1239,17 +1253,17 @@
       <c r="F4">
         <v>4444</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1270,12 +1284,12 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="30.7272727272727" customWidth="1"/>
-    <col min="2" max="2" width="16.2727272727273" customWidth="1"/>
+    <col min="1" max="1" width="30.7238095238095" customWidth="1"/>
+    <col min="2" max="2" width="16.2761904761905" customWidth="1"/>
     <col min="3" max="3" width="41" customWidth="1"/>
-    <col min="4" max="5" width="21.2727272727273" customWidth="1"/>
+    <col min="4" max="5" width="21.2761904761905" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1293,8 +1307,8 @@
       <c r="B2">
         <v>20</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1311,46 +1325,46 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="17.9090909090909" customWidth="1"/>
-    <col min="2" max="2" width="8.63636363636364" customWidth="1"/>
-    <col min="3" max="3" width="7.18181818181818" customWidth="1"/>
+    <col min="1" max="1" width="17.9047619047619" customWidth="1"/>
+    <col min="2" max="2" width="8.63809523809524" customWidth="1"/>
+    <col min="3" max="3" width="7.18095238095238" customWidth="1"/>
     <col min="4" max="4" width="6" customWidth="1"/>
-    <col min="5" max="5" width="9.09090909090909" customWidth="1"/>
-    <col min="6" max="6" width="11.8181818181818" customWidth="1"/>
-    <col min="7" max="7" width="8.63636363636364" customWidth="1"/>
-    <col min="8" max="8" width="14.7272727272727" customWidth="1"/>
-    <col min="9" max="9" width="8.18181818181818" customWidth="1"/>
-    <col min="10" max="10" width="21.4545454545455" customWidth="1"/>
+    <col min="5" max="5" width="9.09523809523809" customWidth="1"/>
+    <col min="6" max="6" width="11.8190476190476" customWidth="1"/>
+    <col min="7" max="7" width="8.63809523809524" customWidth="1"/>
+    <col min="8" max="8" width="14.7238095238095" customWidth="1"/>
+    <col min="9" max="9" width="8.18095238095238" customWidth="1"/>
+    <col min="10" max="10" width="21.4571428571429" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>33</v>
       </c>
       <c r="J1" t="s">
@@ -1373,7 +1387,7 @@
       <c r="E2">
         <v>1234</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="G2">
@@ -1385,7 +1399,7 @@
       <c r="I2">
         <v>20</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="7" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1404,13 +1418,13 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="16.2727272727273" customWidth="1"/>
-    <col min="2" max="2" width="21.2727272727273" customWidth="1"/>
-    <col min="3" max="3" width="18.6363636363636" customWidth="1"/>
+    <col min="1" max="1" width="16.2761904761905" customWidth="1"/>
+    <col min="2" max="2" width="21.2761904761905" customWidth="1"/>
+    <col min="3" max="3" width="18.6380952380952" customWidth="1"/>
     <col min="4" max="4" width="41" customWidth="1"/>
-    <col min="5" max="5" width="19.3636363636364" customWidth="1"/>
+    <col min="5" max="5" width="19.3619047619048" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1434,10 +1448,10 @@
       <c r="A2">
         <v>20</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>43</v>
       </c>
       <c r="D2" t="s">
@@ -1462,7 +1476,7 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
   </cols>
@@ -1481,4 +1495,86 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="7"/>
+  <cols>
+    <col min="8" max="8" width="30.7142857142857" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="H2" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3">
+        <v>4444</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
implementing apply for a lon test case & doing some refactor
</commit_message>
<xml_diff>
--- a/Data Files/Test data.xlsx
+++ b/Data Files/Test data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180" activeTab="5"/>
+    <workbookView windowWidth="28800" windowHeight="12180" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sign up" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,8 @@
     <sheet name="Find transaction" sheetId="4" r:id="rId4"/>
     <sheet name="Open new account" sheetId="5" r:id="rId5"/>
     <sheet name="Update profile info" sheetId="6" r:id="rId6"/>
+    <sheet name="Apply for a Loan" sheetId="7" r:id="rId7"/>
+    <sheet name="Transfer fund" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
   <si>
     <t>First Name</t>
   </si>
@@ -67,6 +69,9 @@
     <t>Confirm</t>
   </si>
   <si>
+    <t>Sign up_Success message</t>
+  </si>
+  <si>
     <t>Mahmoud</t>
   </si>
   <si>
@@ -85,18 +90,90 @@
     <t>0564411666</t>
   </si>
   <si>
-    <t>testuser5</t>
+    <t>testuser8</t>
   </si>
   <si>
     <t>510520@Mm</t>
   </si>
   <si>
+    <t>Your account was created successfully. You are now logged in.</t>
+  </si>
+  <si>
+    <t>End point</t>
+  </si>
+  <si>
+    <t>https://parabank.parasoft.com/</t>
+  </si>
+  <si>
+    <t>Payee Name</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Verify Account</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Sucees Message</t>
+  </si>
+  <si>
+    <t>Mahmoud Elsayed</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>0564151658</t>
+  </si>
+  <si>
+    <t>Bill Payment Complete</t>
+  </si>
+  <si>
+    <t>Transfer amount</t>
+  </si>
+  <si>
+    <t>Transaction date from</t>
+  </si>
+  <si>
+    <t>Transaction date to</t>
+  </si>
+  <si>
+    <t>Account Created Success Message</t>
+  </si>
+  <si>
+    <t>Transtion result text</t>
+  </si>
+  <si>
+    <t>4/28/2025</t>
+  </si>
+  <si>
+    <t>4/29/2025</t>
+  </si>
+  <si>
+    <t>Congratulations, your account is now open.</t>
+  </si>
+  <si>
+    <t>Transaction Results</t>
+  </si>
+  <si>
+    <t>Account created success message</t>
+  </si>
+  <si>
+    <t>Update info_success message</t>
+  </si>
+  <si>
     <t>ahmed</t>
   </si>
   <si>
     <t>ali</t>
   </si>
   <si>
+    <t>Profile Updated</t>
+  </si>
+  <si>
     <t>mohamed</t>
   </si>
   <si>
@@ -109,76 +186,25 @@
     <t>Cairo</t>
   </si>
   <si>
-    <t>state</t>
-  </si>
-  <si>
     <t>0564411611</t>
   </si>
   <si>
-    <t>End point</t>
-  </si>
-  <si>
-    <t>Transfer amount</t>
-  </si>
-  <si>
-    <t>https://parabank.parasoft.com/</t>
-  </si>
-  <si>
-    <t>Payee Name</t>
-  </si>
-  <si>
-    <t>Account</t>
-  </si>
-  <si>
-    <t>Verify Account</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>Sucees Message</t>
-  </si>
-  <si>
-    <t>Mahmoud Elsayed</t>
-  </si>
-  <si>
-    <t>0564151658</t>
-  </si>
-  <si>
-    <t>Bill Payment Complete</t>
-  </si>
-  <si>
-    <t>Transaction date from</t>
-  </si>
-  <si>
-    <t>Transaction date to</t>
-  </si>
-  <si>
-    <t>Account Created Success Message</t>
-  </si>
-  <si>
-    <t>Transtion result text</t>
-  </si>
-  <si>
-    <t>4/28/2025</t>
-  </si>
-  <si>
-    <t>4/29/2025</t>
-  </si>
-  <si>
-    <t>Congratulations, your account is now open.</t>
-  </si>
-  <si>
-    <t>Transaction Results</t>
-  </si>
-  <si>
-    <t>Account created success message</t>
-  </si>
-  <si>
-    <t>Update info_success message</t>
-  </si>
-  <si>
-    <t>Profile Updated</t>
+    <t>Loan amount</t>
+  </si>
+  <si>
+    <t>Down payment</t>
+  </si>
+  <si>
+    <t>Apply for load_Success message</t>
+  </si>
+  <si>
+    <t>Congratulations, your loan has been approved.</t>
+  </si>
+  <si>
+    <t>Transfer fund_success message</t>
+  </si>
+  <si>
+    <t>Transfer Complete!</t>
   </si>
 </sst>
 </file>
@@ -191,13 +217,19 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -675,144 +707,147 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1133,10 +1168,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:G4"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6"/>
@@ -1150,120 +1185,105 @@
     <col min="7" max="7" width="11.8190476190476" customWidth="1"/>
     <col min="8" max="8" width="8.54285714285714" customWidth="1"/>
     <col min="9" max="9" width="10.2761904761905" customWidth="1"/>
-    <col min="10" max="10" width="10" customWidth="1"/>
-    <col min="11" max="11" width="8.36190476190476" customWidth="1"/>
+    <col min="10" max="11" width="13.1428571428571" customWidth="1"/>
+    <col min="12" max="12" width="61.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="2" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2">
         <v>1234</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>16</v>
+      <c r="G2" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="H2">
         <v>1326465</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>18</v>
+      <c r="J2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4">
-        <v>4444</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>26</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1281,7 +1301,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B1" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
@@ -1292,23 +1312,17 @@
     <col min="4" max="5" width="21.2761904761905" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2">
-        <v>20</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+        <v>22</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1340,55 +1354,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>33</v>
+      <c r="G1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="J1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E2">
         <v>1234</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>36</v>
+      <c r="F2" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="G2">
         <v>12345</v>
@@ -1399,8 +1413,8 @@
       <c r="I2">
         <v>20</v>
       </c>
-      <c r="J2" s="7" t="s">
-        <v>37</v>
+      <c r="J2" s="8" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1415,7 +1429,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="N5" sqref="N5:N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
@@ -1429,36 +1443,36 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
         <v>20</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>43</v>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1472,8 +1486,8 @@
   <sheetPr/>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1483,12 +1497,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1502,7 +1516,7 @@
   <sheetPr/>
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
@@ -1512,65 +1526,146 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="H2" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="H2" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>24</v>
+      <c r="D3" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F3">
         <v>4444</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>26</v>
+      <c r="G3" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="13.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="15.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="46.8571428571429" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>50</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="16.8571428571429" customWidth="1"/>
+    <col min="2" max="2" width="31.5714285714286" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implement site map test case
</commit_message>
<xml_diff>
--- a/Data Files/Test data.xlsx
+++ b/Data Files/Test data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6800" firstSheet="4" activeTab="8"/>
+    <workbookView windowWidth="19200" windowHeight="6780"/>
   </bookViews>
   <sheets>
     <sheet name="Sign up" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="Apply for a Loan" sheetId="7" r:id="rId7"/>
     <sheet name="Transfer fund" sheetId="8" r:id="rId8"/>
     <sheet name="Customer Care" sheetId="9" r:id="rId9"/>
+    <sheet name="Parasoft Forums" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="70">
   <si>
     <t>First Name</t>
   </si>
@@ -91,7 +92,7 @@
     <t>0564411666</t>
   </si>
   <si>
-    <t>testuser11</t>
+    <t>testuser16</t>
   </si>
   <si>
     <t>510520@Mm</t>
@@ -230,6 +231,21 @@
   </si>
   <si>
     <t>automation test purpose</t>
+  </si>
+  <si>
+    <t>Thank you Mahmoud Elsayed</t>
+  </si>
+  <si>
+    <t>Site link</t>
+  </si>
+  <si>
+    <t>Parasoft heading</t>
+  </si>
+  <si>
+    <t>https://forums.parasoft.com/</t>
+  </si>
+  <si>
+    <t>Parasoft Forums</t>
   </si>
 </sst>
 </file>
@@ -864,7 +880,7 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1196,23 +1212,23 @@
   <sheetPr/>
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="10.7272727272727" customWidth="1"/>
-    <col min="3" max="3" width="8.63636363636364" customWidth="1"/>
-    <col min="4" max="4" width="4.90909090909091" customWidth="1"/>
+    <col min="2" max="2" width="10.7238095238095" customWidth="1"/>
+    <col min="3" max="3" width="8.63809523809524" customWidth="1"/>
+    <col min="4" max="4" width="4.90476190476191" customWidth="1"/>
     <col min="5" max="5" width="6" customWidth="1"/>
-    <col min="6" max="6" width="9.09090909090909" customWidth="1"/>
-    <col min="7" max="7" width="11.8181818181818" customWidth="1"/>
-    <col min="8" max="8" width="8.54545454545454" customWidth="1"/>
-    <col min="9" max="9" width="10.2727272727273" customWidth="1"/>
-    <col min="10" max="11" width="13.1454545454545" customWidth="1"/>
-    <col min="12" max="12" width="61.5727272727273" customWidth="1"/>
+    <col min="6" max="6" width="9.09523809523809" customWidth="1"/>
+    <col min="7" max="7" width="11.8190476190476" customWidth="1"/>
+    <col min="8" max="8" width="8.54285714285714" customWidth="1"/>
+    <col min="9" max="9" width="10.2761904761905" customWidth="1"/>
+    <col min="10" max="11" width="13.1428571428571" customWidth="1"/>
+    <col min="12" max="12" width="61.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1317,6 +1333,43 @@
     <hyperlink ref="K2" r:id="rId1" display="510520@Mm"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="29.8571428571429" customWidth="1"/>
+    <col min="2" max="2" width="17.2857142857143" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -1330,12 +1383,12 @@
       <selection activeCell="B1" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="30.7272727272727" customWidth="1"/>
-    <col min="2" max="2" width="16.2727272727273" customWidth="1"/>
+    <col min="1" max="1" width="30.7238095238095" customWidth="1"/>
+    <col min="2" max="2" width="16.2761904761905" customWidth="1"/>
     <col min="3" max="3" width="41" customWidth="1"/>
-    <col min="4" max="5" width="21.2727272727273" customWidth="1"/>
+    <col min="4" max="5" width="21.2761904761905" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1365,18 +1418,18 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="17.9090909090909" customWidth="1"/>
-    <col min="2" max="2" width="8.63636363636364" customWidth="1"/>
-    <col min="3" max="3" width="7.18181818181818" customWidth="1"/>
+    <col min="1" max="1" width="17.9047619047619" customWidth="1"/>
+    <col min="2" max="2" width="8.63809523809524" customWidth="1"/>
+    <col min="3" max="3" width="7.18095238095238" customWidth="1"/>
     <col min="4" max="4" width="6" customWidth="1"/>
-    <col min="5" max="5" width="9.09090909090909" customWidth="1"/>
-    <col min="6" max="6" width="11.8181818181818" customWidth="1"/>
-    <col min="7" max="7" width="8.63636363636364" customWidth="1"/>
-    <col min="8" max="8" width="14.7272727272727" customWidth="1"/>
-    <col min="9" max="9" width="8.18181818181818" customWidth="1"/>
-    <col min="10" max="10" width="21.4545454545455" customWidth="1"/>
+    <col min="5" max="5" width="9.09523809523809" customWidth="1"/>
+    <col min="6" max="6" width="11.8190476190476" customWidth="1"/>
+    <col min="7" max="7" width="8.63809523809524" customWidth="1"/>
+    <col min="8" max="8" width="14.7238095238095" customWidth="1"/>
+    <col min="9" max="9" width="8.18095238095238" customWidth="1"/>
+    <col min="10" max="10" width="21.4571428571429" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1458,13 +1511,13 @@
       <selection activeCell="N5" sqref="N5:N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="16.2727272727273" customWidth="1"/>
-    <col min="2" max="2" width="21.2727272727273" customWidth="1"/>
-    <col min="3" max="3" width="18.6363636363636" customWidth="1"/>
+    <col min="1" max="1" width="16.2761904761905" customWidth="1"/>
+    <col min="2" max="2" width="21.2761904761905" customWidth="1"/>
+    <col min="3" max="3" width="18.6380952380952" customWidth="1"/>
     <col min="4" max="4" width="41" customWidth="1"/>
-    <col min="5" max="5" width="19.3636363636364" customWidth="1"/>
+    <col min="5" max="5" width="19.3619047619048" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1516,7 +1569,7 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
   </cols>
@@ -1546,9 +1599,9 @@
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="7"/>
   <cols>
-    <col min="8" max="8" width="30.7181818181818" customWidth="1"/>
+    <col min="8" max="8" width="30.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1628,11 +1681,11 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="13.4272727272727" customWidth="1"/>
-    <col min="2" max="2" width="15.5727272727273" customWidth="1"/>
-    <col min="3" max="3" width="46.8545454545455" customWidth="1"/>
+    <col min="1" max="1" width="13.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="15.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="46.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1672,10 +1725,10 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="16.8545454545455" customWidth="1"/>
-    <col min="2" max="2" width="31.5727272727273" customWidth="1"/>
+    <col min="1" max="1" width="16.8571428571429" customWidth="1"/>
+    <col min="2" max="2" width="31.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1705,17 +1758,17 @@
   <sheetPr/>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="17.9090909090909" customWidth="1"/>
-    <col min="2" max="2" width="34.2727272727273" customWidth="1"/>
-    <col min="3" max="3" width="16.1818181818182" customWidth="1"/>
-    <col min="4" max="4" width="23.7272727272727" customWidth="1"/>
-    <col min="5" max="5" width="30.9090909090909" customWidth="1"/>
+    <col min="1" max="1" width="17.9047619047619" customWidth="1"/>
+    <col min="2" max="2" width="34.2761904761905" customWidth="1"/>
+    <col min="3" max="3" width="16.1809523809524" customWidth="1"/>
+    <col min="4" max="4" width="23.7238095238095" customWidth="1"/>
+    <col min="5" max="5" width="30.9047619047619" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1735,7 +1788,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1747,6 +1800,9 @@
       </c>
       <c r="D2" t="s">
         <v>64</v>
+      </c>
+      <c r="E2" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on site map TC
</commit_message>
<xml_diff>
--- a/Data Files/Test data.xlsx
+++ b/Data Files/Test data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6780"/>
+    <workbookView windowWidth="28800" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Sign up" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
     <t>0564411666</t>
   </si>
   <si>
-    <t>testuser16</t>
+    <t>testuser26</t>
   </si>
   <si>
     <t>510520@Mm</t>
@@ -878,7 +878,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -889,7 +889,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1288,7 +1287,7 @@
       <c r="F2">
         <v>1234</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>17</v>
       </c>
       <c r="H2">
@@ -1300,7 +1299,7 @@
       <c r="J2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L2" t="s">
@@ -1480,7 +1479,7 @@
       <c r="E2">
         <v>1234</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>30</v>
       </c>
       <c r="G2">
@@ -1492,7 +1491,7 @@
       <c r="I2">
         <v>20</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="8" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1662,7 +1661,7 @@
       <c r="F3">
         <v>4444</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1795,7 +1794,7 @@
       <c r="B2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>63</v>
       </c>
       <c r="D2" t="s">

</xml_diff>

<commit_message>
implementing some test cases like (products & locations)
</commit_message>
<xml_diff>
--- a/Data Files/Test data.xlsx
+++ b/Data Files/Test data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180"/>
+    <workbookView windowWidth="19200" windowHeight="6780"/>
   </bookViews>
   <sheets>
     <sheet name="Sign up" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,8 @@
     <sheet name="Transfer fund" sheetId="8" r:id="rId8"/>
     <sheet name="Customer Care" sheetId="9" r:id="rId9"/>
     <sheet name="Parasoft Forums" sheetId="10" r:id="rId10"/>
+    <sheet name="Locations" sheetId="11" r:id="rId11"/>
+    <sheet name="Products" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="78">
   <si>
     <t>First Name</t>
   </si>
@@ -92,7 +94,7 @@
     <t>0564411666</t>
   </si>
   <si>
-    <t>testuser26</t>
+    <t>testuser33</t>
   </si>
   <si>
     <t>510520@Mm</t>
@@ -246,6 +248,30 @@
   </si>
   <si>
     <t>Parasoft Forums</t>
+  </si>
+  <si>
+    <t>location site link</t>
+  </si>
+  <si>
+    <t>Location  site heading</t>
+  </si>
+  <si>
+    <t>https://www.parasoft.com/solutions/</t>
+  </si>
+  <si>
+    <t>Deliver High-Quality &amp; Secure Software</t>
+  </si>
+  <si>
+    <t>Productss site link</t>
+  </si>
+  <si>
+    <t>Products site heading</t>
+  </si>
+  <si>
+    <t>https://www.parasoft.com/products/</t>
+  </si>
+  <si>
+    <t>Products</t>
   </si>
 </sst>
 </file>
@@ -878,8 +904,9 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1231,37 +1258,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
       <c r="L1" t="s">
@@ -1269,16 +1296,16 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E2" t="s">
@@ -1287,7 +1314,7 @@
       <c r="F2">
         <v>1234</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="9" t="s">
         <v>17</v>
       </c>
       <c r="H2">
@@ -1296,10 +1323,10 @@
       <c r="I2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L2" t="s">
@@ -1307,24 +1334,24 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1342,7 +1369,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A1" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1368,6 +1395,86 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="38.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="39.5714285714286" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://www.parasoft.com/solutions/" tooltip="https://www.parasoft.com/solutions/"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="37.8571428571429" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://www.parasoft.com/products/"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -1399,8 +1506,8 @@
       <c r="A2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1432,31 +1539,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>26</v>
       </c>
       <c r="J1" t="s">
@@ -1479,7 +1586,7 @@
       <c r="E2">
         <v>1234</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="9" t="s">
         <v>30</v>
       </c>
       <c r="G2">
@@ -1491,7 +1598,7 @@
       <c r="I2">
         <v>20</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="9" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1540,10 +1647,10 @@
       <c r="A2">
         <v>20</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>38</v>
       </c>
       <c r="D2" t="s">
@@ -1604,55 +1711,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="H2" s="5" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="H2" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E3" t="s">
@@ -1661,7 +1768,7 @@
       <c r="F3">
         <v>4444</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="9" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1742,7 +1849,7 @@
       <c r="A2">
         <v>20</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1791,10 +1898,10 @@
       <c r="A2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>63</v>
       </c>
       <c r="D2" t="s">

</xml_diff>

<commit_message>
implementing (forgot logon info) test case
</commit_message>
<xml_diff>
--- a/Data Files/Test data.xlsx
+++ b/Data Files/Test data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6780"/>
+    <workbookView windowWidth="28800" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Sign up" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
     <t>0564411666</t>
   </si>
   <si>
-    <t>testuser33</t>
+    <t>testuser1</t>
   </si>
   <si>
     <t>510520@Mm</t>
@@ -906,7 +906,7 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1239,7 +1239,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6"/>
@@ -1702,7 +1702,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="7"/>

</xml_diff>